<commit_message>
edit personal excel, add clk and rst signals in datapath diagram
</commit_message>
<xml_diff>
--- a/Personal Logs/1120203053.xlsx
+++ b/Personal Logs/1120203053.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86159\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitLocal\BIT-pipelined-cpu\Personal Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4699C13E-4960-4254-8F83-917B21FC3A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B1BFA1-413D-4348-978B-3BA532FDE6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,43 +47,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>T1：XXXXXXXXXXXXXXXX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T2:  XXXXXXXXXXXXXXXX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T3:  XXXXXXXXXXXXXXXX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T1：XXXXXXXXXXXXXXXX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q1：XXXXXXXXXXXXXXXX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q2：XXXXXXXXXXXXXXXX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q3：XXXXXXXXXXXXXXXX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A1：Q1的解决办法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A3：Q3的解决办法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A2：Q2的解决办法</t>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>听课，学习CPU的功能和基本结构，重温指令执行过程与数据通路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>团队协商，各自了解不同指令集异同与优劣，确定以单周期CPU-流水线CPU-编写程序接口-上板的流程完成实验。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>听课，深入了解指令执行方案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>团队协商，分享学习心得，确定选择MIPS指令集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对单周期CPU进行分工协作，我负责指令译码部分工作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>仔细挑选要实现的子指令集，优先编写需求与设计文档</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据MIPS文档，</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -475,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -509,262 +501,270 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>44431</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E2" s="9">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="8">
+        <v>44432</v>
+      </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>44433</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
-        <v>44432</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="9">
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9">
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
-        <v>44433</v>
+        <v>44434</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="9">
-        <v>0.2</v>
-      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="10"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
-      <c r="B10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="10"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
+      <c r="A11" s="8">
+        <v>44435</v>
+      </c>
       <c r="B11" s="3"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="3"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="3"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
+      <c r="A14" s="8">
+        <v>44436</v>
+      </c>
       <c r="B14" s="3"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="3"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="3"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
+      <c r="A17" s="8">
+        <v>44437</v>
+      </c>
       <c r="B17" s="3"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="3"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="3"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
+      <c r="A20" s="8">
+        <v>44438</v>
+      </c>
       <c r="B20" s="3"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="3"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="3"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
+      <c r="A23" s="8">
+        <v>44439</v>
+      </c>
       <c r="B23" s="3"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="3"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="A25" s="8"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="A26" s="8">
+        <v>44440</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="A27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
+        <v>44441</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="E5:E7"/>
+  <mergeCells count="14">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
edit personal log of lhy
</commit_message>
<xml_diff>
--- a/Personal Logs/1120203053.xlsx
+++ b/Personal Logs/1120203053.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitLocal\BIT-pipelined-cpu\Personal Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B1BFA1-413D-4348-978B-3BA532FDE6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69BFA72-F166-423F-AB7E-1892286A918D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="41">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,7 +75,119 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>根据MIPS文档，</t>
+    <t>根据MIPS文档，对挑选的指令分析字段组成，进行编码，设计数据通路。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>与队友协同编写信号定义，编写definitions头文件，确定不同指令对应的编码、控制信息。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>确定好接口与模块后，开始编写Verilog代码。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编写寄存器模块、译码器模块、ALU及多路选择器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>继续编写ALU、改进线路，优化了前后阶段的接口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>线路旁路过多，如指令JR的数据不经过ALU，同样向后传递</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将线路整合进ALU中，ALU直接输出ALUInput2的值，可以简化线路与后向接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>与队友交流，根据其他模块的完成情况对负责的模块进行改进优化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经协商确定实现最经典的五阶段流水线，在单周期流水线的基础上改进，我负责模块设计、译码执行、数据通路的绘制工作。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加流水线寄存器，在流水线寄存器处确定了不同阶段的接口，即数据及信号传递。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过流水线寄存器划分开译码阶段与执行阶段。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优化执行阶段代码，使其负载更均衡。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对单周期CPU的数据及信号进行重命名，使其在全局更易区分，以后缀区分不同阶段。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>与队友协商解决流水线冒险的方案，并罗列可能的冒险情况。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我负责在执行阶段实现数据转发功能，并协同队友开发冒险控制模块。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编写数据转发控制模块，并添加更多的数据线路，为ALU的输入添加多路选择器。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>流水线寄存器模块接收冒险控制模块的停顿或刷新信号，以停顿该阶段流水线或刷新数据。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始根据模块图、接口等绘制数据通路图。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>继续绘制数据通路图，与队友交流。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>整合改进后的流水线CPU，进行仿真测试与上板。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编写多个仿真测试程序，以验证CPU正确性。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>继续绘制数据通路图，同时改进流水线CPU代码。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>队友开始设计并编写vga接口，我协同队友完成设计。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>为vga接口提供CPU输出，因此需改进CPU代码，同时编写顶层模块协同CPU与VGA进行通信。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机房验证VGA接口，成功输出CPU内存信息。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>着手编写文档，与队友一起制作答辩PPT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>改进CPU与接口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>答辩。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编写文档。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -128,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -151,11 +263,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -164,27 +326,51 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -467,304 +653,586 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.9140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="43.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="39.08203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="58.9140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.08203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.9140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.08203125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.9140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="A2" s="7">
         <v>44431</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="9">
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="8">
         <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="10"/>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>44432</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="9">
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="8">
         <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="10"/>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>44433</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="9">
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8">
         <v>0.15</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>44434</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>44435</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="A10" s="7">
+        <v>44436</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
-        <v>44435</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
-        <v>44436</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>44437</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>44438</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="17">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>44439</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="17">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="14"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
-        <v>44437</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="A17" s="11">
+        <v>44440</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="8">
-        <v>44438</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A19" s="11">
+        <v>44441</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="17">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A21" s="11">
+        <v>44442</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="17">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="16"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="8">
-        <v>44439</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="A24" s="11">
+        <v>44443</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="17">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="16"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="8">
-        <v>44440</v>
-      </c>
+      <c r="A26" s="11"/>
+      <c r="B26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="14"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="8">
-        <v>44441</v>
+      <c r="A27" s="11">
+        <v>44444</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="17">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="14"/>
+    </row>
+    <row r="29" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A29" s="15">
+        <v>44445</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0.75</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
+      <c r="A30" s="11">
+        <v>44446</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="17">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="14"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="15">
+        <v>44447</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="15">
+        <v>44448</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="17">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="15">
+        <v>44449</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="18"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="15">
+        <v>44450</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="6">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="26">
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
edit lhy's personal log
</commit_message>
<xml_diff>
--- a/Personal Logs/1120203053.xlsx
+++ b/Personal Logs/1120203053.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitLocal\BIT-pipelined-cpu\Personal Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69BFA72-F166-423F-AB7E-1892286A918D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5767A7CA-1609-41E8-B2C4-8EBA8B518E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="53">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,30 +51,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>听课，学习CPU的功能和基本结构，重温指令执行过程与数据通路</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>团队协商，各自了解不同指令集异同与优劣，确定以单周期CPU-流水线CPU-编写程序接口-上板的流程完成实验。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>听课，深入了解指令执行方案</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>团队协商，分享学习心得，确定选择MIPS指令集</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对单周期CPU进行分工协作，我负责指令译码部分工作</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>仔细挑选要实现的子指令集，优先编写需求与设计文档</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>根据MIPS文档，对挑选的指令分析字段组成，进行编码，设计数据通路。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -87,26 +67,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>编写寄存器模块、译码器模块、ALU及多路选择器</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>继续编写ALU、改进线路，优化了前后阶段的接口。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>线路旁路过多，如指令JR的数据不经过ALU，同样向后传递</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>将线路整合进ALU中，ALU直接输出ALUInput2的值，可以简化线路与后向接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>与队友交流，根据其他模块的完成情况对负责的模块进行改进优化</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>经协商确定实现最经典的五阶段流水线，在单周期流水线的基础上改进，我负责模块设计、译码执行、数据通路的绘制工作。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -175,19 +139,103 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>着手编写文档，与队友一起制作答辩PPT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>改进CPU与接口。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>答辩。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>编写文档。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我们对于指令集的选取产生了分歧。我更倾向于选择上学期实现过的RISC-V架构，而队友更推荐MIPS架构。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>团队协商，分享学习心得，确定选择MIPS指令集。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>听课，深入了解指令执行方案。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>听课，学习CPU的功能和基本结构，重温指令执行过程与数据通路。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>仔细挑选要实现的子指令集，优先编写需求与设计文档。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对单周期CPU进行分工协作，我负责指令译码部分工作。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编写寄存器模块、译码器模块、ALU及多路选择器。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>与队友交流，根据其他模块的完成情况对负责的模块进行改进优化。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>着手编写文档，与队友一起制作答辩PPT。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>准备答辩。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将线路整合进ALU中，ALU直接输出ALUInput2的值，可以简化线路与后向接口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>线路旁路过多，如指令JR的数据不经过ALU，同样向后传递。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经过商讨与比较，MIPS架构的可查询资料更多，指令的字段组成更简洁明了，而RISC-V字段包括fnt3、fnt5等，且位置不一，不利于译码模块的编写。最终选择MIPS架构。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>definitions头文件定义不全或不规范，不方便使用。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实际上，definitions头文件在整个开发过程中是在不断修改的，这与我们初始没有进行完善的CPU设计有关。但在不断迭代中，信号定义趋于完善。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如何处理结构冒险？如同时读取与写入寄存器。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我们更改了寄存器模块的代码，使其读取寄存器采用wire直接输出，而寄存器在时钟下降沿才写入，避免了寄存器冲突。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重命名错误或遗漏产生bug。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>信号与数据的重命名是必要的也是繁琐的，清晰的后缀区分更有利于后续流水线的信号传递。但同时，修改信号意味着大量重写代码，即使直接替换也会有遗漏产生。在多次debug与测试后终于解决。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>执行阶段负载过多。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据转发模块设置在执行阶段。执行阶段需先等待转发模块的信号与转发的数据稳定后，ALU才能接收到正确的输入并输出。在缩减模块后，该阶段消耗的时间仍较多。因此在目前的阶段，解决方法只能为CPU降频，经测试，10MHz下CPU表现正常（可能允许的频率更高）；100MHz则会输出错误。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直接跳转与分支预测需停顿一个周期，造成CPU资源浪费。连续指令下的取数-使用冒险与分支跳转产生矛盾，CPU出现未知行为。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>与队友协作，大幅度修改取指阶段，使直接跳转与分支预测的目标指令地址直接产生，并输出给NPC，下一周期可直接取用，以此减少一个周期的浪费。修改冒险控制模块，解决了矛盾。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -337,6 +385,33 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="58" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -344,33 +419,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -655,16 +703,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.9140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.08203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.58203125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="45.58203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.9140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.08203125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.9140625" style="1"/>
@@ -688,41 +735,41 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="A2" s="16">
         <v>44431</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="16"/>
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="8">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="16">
         <v>44432</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
@@ -730,29 +777,29 @@
       <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="17">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:5" ht="66" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+      <c r="A6" s="16">
         <v>44433</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
@@ -760,14 +807,14 @@
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="17">
         <v>0.15</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
@@ -775,14 +822,14 @@
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>44434</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>5</v>
@@ -794,29 +841,29 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>44435</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="E9" s="6">
         <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+      <c r="A10" s="16">
         <v>44436</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -824,14 +871,14 @@
       <c r="D10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="11">
         <v>0.3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
@@ -839,272 +886,272 @@
       <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="14"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>44437</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="E12" s="6">
         <v>0.35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
+    <row r="13" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
         <v>44438</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>44439</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="66" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="15">
+        <v>44440</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+      <c r="B18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
+        <v>44441</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="11">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="1:5" ht="99" x14ac:dyDescent="0.3">
+      <c r="A21" s="15">
+        <v>44442</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="11">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+      <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="17">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="3" t="s">
+      <c r="C22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="15"/>
+      <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="14"/>
-    </row>
-    <row r="15" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
-        <v>44439</v>
-      </c>
-      <c r="B15" s="13" t="s">
+      <c r="C23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="15">
+        <v>44443</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="17">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="3" t="s">
+      <c r="C24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="11">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="15"/>
+      <c r="B25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="15"/>
+      <c r="B26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="15">
+        <v>44444</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="14"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="11">
-        <v>44440</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="17">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A19" s="11">
-        <v>44441</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="C27" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="11">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+      <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="17">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="3" t="s">
+      <c r="C28" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="13"/>
+    </row>
+    <row r="29" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
+        <v>44445</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="14"/>
-    </row>
-    <row r="21" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
-        <v>44442</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="17">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="14"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="11">
-        <v>44443</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="17">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="16"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="14"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
-        <v>44444</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="17">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="14"/>
-    </row>
-    <row r="29" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A29" s="15">
-        <v>44445</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="10" t="s">
+      <c r="C29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="6">
@@ -1112,93 +1159,93 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="11">
+      <c r="A30" s="15">
         <v>44446</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="17">
+        <v>27</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="11">
         <v>0.8</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="14"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="15">
+        <v>38</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="13"/>
+    </row>
+    <row r="32" spans="1:5" ht="66" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
         <v>44447</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="E32" s="6">
         <v>0.85</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="15">
+      <c r="A33" s="8">
         <v>44448</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="17">
+      <c r="C33" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="11">
         <v>0.9</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="15">
+      <c r="A34" s="8">
         <v>44449</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="18"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="12"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="15">
+      <c r="A35" s="8">
         <v>44450</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E35" s="6">
@@ -1207,32 +1254,32 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E27:E28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>